<commit_message>
Minor fixes for computing contributions to EPF/VPF
</commit_message>
<xml_diff>
--- a/src/Tax Simulator.xlsx
+++ b/src/Tax Simulator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrajvir\Documents\Tax Simulator\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F647C739-E914-4D4C-849F-F274388B62E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBEF516-06AB-4E9F-B772-32E4D664F578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{3843DC55-979D-4730-884A-784DB37EFD9C}"/>
   </bookViews>
@@ -354,7 +354,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -375,8 +375,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -735,19 +733,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="63.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.3984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.06640625" style="1"/>
-    <col min="5" max="5" width="11.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.06640625" style="1"/>
     <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.06640625" style="1"/>
@@ -761,11 +759,11 @@
         <v>0</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="E1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -784,13 +782,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2"/>
@@ -811,9 +809,9 @@
         <v>43922</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -833,13 +831,13 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="17">
-        <v>0</v>
-      </c>
-      <c r="F4" s="17">
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15">
         <v>250000</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <v>0</v>
       </c>
       <c r="H4" s="2"/>
@@ -860,13 +858,13 @@
         <v>12</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <v>250000</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="15">
         <v>500000</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="16">
         <v>0.05</v>
       </c>
       <c r="H5" s="2"/>
@@ -883,17 +881,17 @@
       <c r="A6" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="17">
+      <c r="E6" s="15">
         <v>500000</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="15">
         <v>1000000</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="17">
         <v>0.2</v>
       </c>
       <c r="H6" s="2"/>
@@ -914,11 +912,11 @@
         <v>0</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="17">
+      <c r="E7" s="15">
         <v>1000000</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="19">
+      <c r="F7" s="15"/>
+      <c r="G7" s="17">
         <v>0.3</v>
       </c>
       <c r="H7" s="2"/>
@@ -939,9 +937,9 @@
         <v>0</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -960,11 +958,11 @@
         <v>0</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -976,21 +974,21 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="14">
         <f>MIN(B11,MAX(1/4/2020,B3))</f>
         <v>43922</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="2"/>
@@ -1004,16 +1002,16 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <v>44286</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1028,13 +1026,13 @@
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="17">
-        <v>0</v>
-      </c>
-      <c r="F12" s="17">
+      <c r="E12" s="15">
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
         <v>250000</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <v>0</v>
       </c>
       <c r="H12" s="2"/>
@@ -1056,13 +1054,13 @@
         <v>1</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="17">
+      <c r="E13" s="15">
         <v>250000</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="15">
         <v>500000</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="16">
         <v>0.05</v>
       </c>
       <c r="H13" s="2"/>
@@ -1086,13 +1084,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="17">
+      <c r="E14" s="15">
         <v>500000</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="15">
         <v>750000</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="17">
         <v>0.1</v>
       </c>
       <c r="H14" s="2"/>
@@ -1116,13 +1114,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="17">
+      <c r="E15" s="15">
         <v>750000</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="15">
         <v>1000000</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="17">
         <v>0.15</v>
       </c>
       <c r="H15" s="2"/>
@@ -1146,13 +1144,13 @@
         <v>5</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="17">
+      <c r="E16" s="15">
         <v>1000000</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="15">
         <v>1250000</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="17">
         <v>0.2</v>
       </c>
       <c r="H16" s="2"/>
@@ -1176,13 +1174,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="17">
+      <c r="E17" s="15">
         <v>1250000</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="15">
         <v>1500000</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="17">
         <v>0.25</v>
       </c>
       <c r="H17" s="2"/>
@@ -1206,11 +1204,11 @@
         <v>5</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="17">
+      <c r="E18" s="15">
         <v>1500000</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="19">
+      <c r="F18" s="15"/>
+      <c r="G18" s="17">
         <v>0.3</v>
       </c>
       <c r="H18" s="2"/>
@@ -1234,9 +1232,9 @@
         <v>5</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1258,11 +1256,11 @@
         <v>5</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1284,11 +1282,11 @@
         <v>5</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1310,11 +1308,11 @@
         <v>5</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1336,11 +1334,11 @@
         <v>5</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1362,11 +1360,11 @@
         <v>5</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1642,175 +1640,183 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="37" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="37" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="5"/>
+    </row>
     <row r="38" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="13">
-        <f>ROUND((B5/100*B2)*(DATEDIF(B10,B11,"m")+(DATEDIF(B10,B11,"md")/DAY(EOMONTH(B10,0)))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C38" s="13">
-        <f>ROUND((B5/100*B2)*(DATEDIF(B10,B11,"m")+(DATEDIF(B10,B11,"md")/DAY(EOMONTH(B10,0)))),0)</f>
-        <v>0</v>
-      </c>
+      <c r="B38" s="11">
+        <f>ROUND((B5/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND((B5/100*B2)*DATEDIF(B10,B11,"m"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="11">
+        <f>ROUND((B5/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND((B5/100*B2)*DATEDIF(B10,B11,"m"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="13">
-        <f>IF(B7&gt;B5,((B7-B5)/100*B2)*(DATEDIF(B10,B11,"m")+(DATEDIF(B10,B11,"md")/DAY(EOMONTH(B10,0)))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C39" s="13">
-        <f>IF(B7&gt;B5,((B7-B5)/100*B2)*(DATEDIF(B10,B11,"m")+(DATEDIF(B10,B11,"md")/DAY(EOMONTH(B10,0)))),0)</f>
-        <v>0</v>
-      </c>
+      <c r="B39" s="11">
+        <f>IF(B7&gt;B5,ROUND(((B7-B5)/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND(((B7-B5)/100*B2)*DATEDIF(B10,B11,"m"),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="11">
+        <f>IF(B7&gt;B5,ROUND(((B7-B5)/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND(((B7-B5)/100*B2)*DATEDIF(B10,B11,"m"),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="13">
-        <f>ROUND((((DATEDIF(B10,B11,"m")+(DATEDIF(B10,B11,"md")/DAY(EOMONTH(B10,0))))*B1/12)+B4+B8+B9)+IF(B6="Yes",-1*B38,0),2)</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="13">
-        <f>ROUND((((DATEDIF(B10,B11,"m")+(DATEDIF(B10,B11,"md")/DAY(EOMONTH(B10,0))))*B1/12)+B4+B8+B9)+IF(B6="Yes",-1*C38,0),2)</f>
+      <c r="B40" s="11">
+        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*B38,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="11">
+        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*C38,0),0)</f>
         <v>0</v>
       </c>
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="12">
         <v>50000</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="C41" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="12">
         <f>MIN(150000,B18+B38+B39)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="7"/>
+      <c r="C42" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="12">
         <f>MIN(50000,B19)+MIN(25000,B20)+MIN(25000,B21)+MIN(50000,B22)+MIN(75000,B23)+MIN(125000,B24)+MIN(40000,B25)+MIN(100000,B26)+B27+MIN(50000,B28)+MIN(150000,B29)+MIN(150000,B30)+B31+MIN(10000,B32)+MIN(50000,B33)+MIN(75000,B34)+MIN(125000,B35)</f>
         <v>0</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="13">
+      <c r="B45" s="11">
         <f>MAX(0,B40-SUM(B41:B43)-SUM(B14:B17))</f>
         <v>0</v>
       </c>
-      <c r="C45" s="13">
+      <c r="C45" s="11">
         <f>C40</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="14" cm="1">
+      <c r="B46" s="12" cm="1">
         <f t="array" ref="B46">ROUND(IF(B45&gt;500000,SUMPRODUCT(G4:G7-G3:G6,B45-E4:E7,N(B45&gt;E4:E7)),0),2)</f>
         <v>0</v>
       </c>
-      <c r="C46" s="14" cm="1">
+      <c r="C46" s="12" cm="1">
         <f t="array" ref="C46">ROUND(IF(C45&gt;500000,SUMPRODUCT(G12:G18-G11:G17,C45-E12:E18,N(C45&gt;E12:E18)),0),2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="14">
+      <c r="B47" s="12">
         <f>IF(B45&lt;5000000,0,IF(B45&lt;=10000000,0.1*B46,IF(B45&lt;=20000000,0.15*B46,IF(B45&lt;=50000000,0.25*B46,0.37*B46))))</f>
         <v>0</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="12">
         <f>IF(C45&lt;5000000,0,IF(C45&lt;=10000000,0.1*C46,IF(C45&lt;=20000000,0.15*C46,IF(C45&lt;=50000000,0.25*C46,0.37*C46))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="14">
+      <c r="B48" s="12">
         <f>0.04*(B46+B47)</f>
         <v>0</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="12">
         <f>0.04*(C46+C47)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="14">
+      <c r="B49" s="12">
         <f>ROUND(SUM(B46:B48),2)</f>
         <v>0</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="12">
         <f>ROUND(SUM(C46:C48),2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="50" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B51" s="12">
         <f>ROUND(ABS(B49-C49),2)</f>
         <v>0</v>
       </c>
       <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="15" t="str">
+      <c r="B52" s="13" t="str">
         <f>IF(B49&gt;C49,"New Regime", "Old Regime")</f>
         <v>Old Regime</v>
       </c>
       <c r="C52" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7E6eU8uUr/+RFZ4/tShdJ2yM7xtA3cSOIpm+SslUSv2XvTw+YToEo4Jm/gaMYVsGDA+CdFIyh+wnEeoGTVW+3A==" saltValue="CWtbTEwI2mVgCTVzXhqIHQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DcJTmxNFHV7jlQvrkyJ3/Js/9TJjK4VQdmMvRvO7UyZDSUI1YbALtu7DC9KNv1qXi5fdEN6mriAUebX1Z4/vmQ==" saltValue="17q9ZWIZw5r7j2bNOc0htQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A50:XFD50"/>
   </mergeCells>

</xml_diff>

<commit_message>
Including tax benefits under Section 10 and Section 24
</commit_message>
<xml_diff>
--- a/src/Tax Simulator.xlsx
+++ b/src/Tax Simulator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrajvir\Documents\Tax Simulator\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBEF516-06AB-4E9F-B772-32E4D664F578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C3B60-FF3A-4021-B85D-5E08877CCDF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{3843DC55-979D-4730-884A-784DB37EFD9C}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Old Regime</t>
   </si>
@@ -231,6 +231,21 @@
   </si>
   <si>
     <t>VPF Contribution (%)</t>
+  </si>
+  <si>
+    <t>Loss from House Property</t>
+  </si>
+  <si>
+    <t>Deductions under loss from house property</t>
+  </si>
+  <si>
+    <t>Section 10 (Deductions allowed only in Old Regime, excluding Section 10(14))</t>
+  </si>
+  <si>
+    <t>Section 10(14) deductions (allowances exempted in both the tax regimes)</t>
+  </si>
+  <si>
+    <t>Section 10 deductions</t>
   </si>
 </sst>
 </file>
@@ -354,7 +369,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -367,9 +382,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
@@ -410,7 +422,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent3" xfId="5" builtinId="37"/>
@@ -731,15 +750,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA4E777-56A7-4B35-9A19-002DF34E045D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="63.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.46484375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.3984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.1328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.06640625" style="1"/>
@@ -752,18 +771,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1">
         <v>0</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="E1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -775,20 +794,20 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2"/>
@@ -802,16 +821,16 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="3">
         <v>43922</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -823,7 +842,7 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4">
@@ -831,13 +850,13 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="15">
-        <v>0</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
         <v>250000</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <v>0</v>
       </c>
       <c r="H4" s="2"/>
@@ -851,20 +870,20 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>12</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>250000</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>500000</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <v>0.05</v>
       </c>
       <c r="H5" s="2"/>
@@ -878,20 +897,20 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>500000</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>1000000</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="16">
         <v>0.2</v>
       </c>
       <c r="H6" s="2"/>
@@ -905,18 +924,18 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>1000000</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="17">
+      <c r="F7" s="14"/>
+      <c r="G7" s="16">
         <v>0.3</v>
       </c>
       <c r="H7" s="2"/>
@@ -930,16 +949,16 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -951,18 +970,18 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -974,21 +993,21 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <f>MIN(B11,MAX(1/4/2020,B3))</f>
         <v>43922</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="2"/>
@@ -1002,16 +1021,16 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>44286</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1026,13 +1045,13 @@
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="15">
-        <v>0</v>
-      </c>
-      <c r="F12" s="15">
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14">
         <v>250000</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="15">
         <v>0</v>
       </c>
       <c r="H12" s="2"/>
@@ -1050,17 +1069,17 @@
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>250000</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>500000</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <v>0.05</v>
       </c>
       <c r="H13" s="2"/>
@@ -1074,23 +1093,23 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>500000</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>750000</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="16">
         <v>0.1</v>
       </c>
       <c r="H14" s="2"/>
@@ -1104,23 +1123,23 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>750000</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>1000000</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="16">
         <v>0.15</v>
       </c>
       <c r="H15" s="2"/>
@@ -1134,23 +1153,23 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>1000000</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>1250000</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="16">
         <v>0.2</v>
       </c>
       <c r="H16" s="2"/>
@@ -1164,23 +1183,23 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>1250000</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>1500000</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="16">
         <v>0.25</v>
       </c>
       <c r="H17" s="2"/>
@@ -1194,21 +1213,21 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <v>1500000</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="17">
+      <c r="F18" s="14"/>
+      <c r="G18" s="16">
         <v>0.3</v>
       </c>
       <c r="H18" s="2"/>
@@ -1222,19 +1241,19 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1246,21 +1265,21 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1272,21 +1291,21 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1298,21 +1317,21 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1324,21 +1343,21 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1350,21 +1369,21 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1376,13 +1395,13 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
@@ -1400,13 +1419,13 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="2"/>
@@ -1424,13 +1443,13 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="2"/>
@@ -1448,13 +1467,13 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="2"/>
@@ -1472,19 +1491,19 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="7"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1496,13 +1515,13 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="2"/>
@@ -1520,13 +1539,13 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="2"/>
@@ -1544,13 +1563,13 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="2"/>
@@ -1568,13 +1587,13 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="2"/>
@@ -1592,13 +1611,13 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="2"/>
@@ -1616,13 +1635,13 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="2"/>
@@ -1641,186 +1660,244 @@
     </row>
     <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="37" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="5"/>
+      <c r="A37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="20">
+        <v>0</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="20">
+        <v>0</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="22">
+        <v>0</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B41" s="10">
         <f>ROUND((B5/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND((B5/100*B2)*DATEDIF(B10,B11,"m"),0)</f>
         <v>0</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C41" s="10">
         <f>ROUND((B5/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND((B5/100*B2)*DATEDIF(B10,B11,"m"),0)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="19" t="s">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B42" s="10">
         <f>IF(B7&gt;B5,ROUND(((B7-B5)/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND(((B7-B5)/100*B2)*DATEDIF(B10,B11,"m"),0),0)</f>
         <v>0</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C42" s="10">
         <f>IF(B7&gt;B5,ROUND(((B7-B5)/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND(((B7-B5)/100*B2)*DATEDIF(B10,B11,"m"),0),0)</f>
         <v>0</v>
       </c>
-      <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="19" t="s">
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="11">
-        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*B38,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="11">
-        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*C38,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="19" t="s">
+      <c r="B43" s="10">
+        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*B41,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="10">
+        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*C41,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B44" s="11">
         <v>50000</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="19" t="s">
+      <c r="C44" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="12">
-        <f>MIN(150000,B18+B38+B39)</f>
-        <v>0</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="19" t="s">
+      <c r="B45" s="11">
+        <f>MIN(150000,B18+B41+B42)</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B46" s="11">
         <f>MIN(50000,B19)+MIN(25000,B20)+MIN(25000,B21)+MIN(50000,B22)+MIN(75000,B23)+MIN(125000,B24)+MIN(40000,B25)+MIN(100000,B26)+B27+MIN(50000,B28)+MIN(150000,B29)+MIN(150000,B30)+B31+MIN(10000,B32)+MIN(50000,B33)+MIN(75000,B34)+MIN(125000,B35)</f>
         <v>0</v>
       </c>
-      <c r="C43" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="19" t="s">
+      <c r="C46" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="11">
+        <f>MIN(200000,B37)</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="11">
+        <f>SUM(B38:B39)</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="12">
+        <f>C39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="11">
-        <f>MAX(0,B40-SUM(B41:B43)-SUM(B14:B17))</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="11">
-        <f>C40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="19" t="s">
+      <c r="B50" s="10">
+        <f>MAX(0,B43-SUM(B44:B48)-SUM(B14:B17))</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="10">
+        <f>MAX(0,C43-C48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="12" cm="1">
-        <f t="array" ref="B46">ROUND(IF(B45&gt;500000,SUMPRODUCT(G4:G7-G3:G6,B45-E4:E7,N(B45&gt;E4:E7)),0),2)</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="12" cm="1">
-        <f t="array" ref="C46">ROUND(IF(C45&gt;500000,SUMPRODUCT(G12:G18-G11:G17,C45-E12:E18,N(C45&gt;E12:E18)),0),2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="19" t="s">
+      <c r="B51" s="11" cm="1">
+        <f t="array" ref="B51">ROUND(IF(B50&gt;500000,SUMPRODUCT(G4:G7-G3:G6,B50-E4:E7,N(B50&gt;E4:E7)),0),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="11" cm="1">
+        <f t="array" ref="C51">ROUND(IF(C50&gt;500000,SUMPRODUCT(G12:G18-G11:G17,C50-E12:E18,N(C50&gt;E12:E18)),0),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="12">
-        <f>IF(B45&lt;5000000,0,IF(B45&lt;=10000000,0.1*B46,IF(B45&lt;=20000000,0.15*B46,IF(B45&lt;=50000000,0.25*B46,0.37*B46))))</f>
-        <v>0</v>
-      </c>
-      <c r="C47" s="12">
-        <f>IF(C45&lt;5000000,0,IF(C45&lt;=10000000,0.1*C46,IF(C45&lt;=20000000,0.15*C46,IF(C45&lt;=50000000,0.25*C46,0.37*C46))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="19" t="s">
+      <c r="B52" s="11">
+        <f>IF(B50&lt;5000000,0,IF(B50&lt;=10000000,0.1*B51,IF(B50&lt;=20000000,0.15*B51,IF(B50&lt;=50000000,0.25*B51,0.37*B51))))</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="11">
+        <f>IF(C50&lt;5000000,0,IF(C50&lt;=10000000,0.1*C51,IF(C50&lt;=20000000,0.15*C51,IF(C50&lt;=50000000,0.25*C51,0.37*C51))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="12">
-        <f>0.04*(B46+B47)</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="12">
-        <f>0.04*(C46+C47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="19" t="s">
+      <c r="B53" s="11">
+        <f>0.04*(B51+B52)</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="11">
+        <f>0.04*(C51+C52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="12">
-        <f>ROUND(SUM(B46:B48),2)</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="12">
-        <f>ROUND(SUM(C46:C48),2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A51" s="20" t="s">
+      <c r="B54" s="11">
+        <f>ROUND(SUM(B51:B53),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="11">
+        <f>ROUND(SUM(C51:C53),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A56" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="12">
-        <f>ROUND(ABS(B49-C49),2)</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" s="20" t="s">
+      <c r="B56" s="11">
+        <f>ROUND(ABS(B54-C54),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A57" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="13" t="str">
-        <f>IF(B49&gt;C49,"New Regime", "Old Regime")</f>
+      <c r="B57" s="12" t="str">
+        <f>IF(B54&gt;C54,"New Regime", "Old Regime")</f>
         <v>Old Regime</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C57" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DcJTmxNFHV7jlQvrkyJ3/Js/9TJjK4VQdmMvRvO7UyZDSUI1YbALtu7DC9KNv1qXi5fdEN6mriAUebX1Z4/vmQ==" saltValue="17q9ZWIZw5r7j2bNOc0htQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rwmyt6hHFpYmvFLcvmcX67p6pfpbl+rOXDJj/5Rs0Rz96jO2/hYXq6KmCdxUW8xLjBKV6kIhqWWw+5ZMJQpJIQ==" saltValue="iq/Ekhjv1Lh2pW3nyEiDOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A50:XFD50"/>
+    <mergeCell ref="A55:XFD55"/>
   </mergeCells>
-  <dataValidations xWindow="794" yWindow="922" count="14">
+  <dataValidations xWindow="794" yWindow="922" count="17">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Housing Loan Benefit" error="Section 80EEA benefit is applicable only when benefit is not claimed under Section 80EE._x000a_" sqref="B29" xr:uid="{9996CA8A-1186-40D8-8322-5EEC3D7CD6F5}">
       <formula1>$B$28=0</formula1>
     </dataValidation>
@@ -1862,6 +1939,9 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Housing loan benefit" error="Section 80EEA benefit is applicable only when benefit is not claimed under Section 80EE._x000a_" sqref="B28" xr:uid="{F90C388A-3E0D-4710-A78E-B724F22E5850}">
       <formula1>$B$29=0</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Loss from House Property" prompt="Deductions under loss of income due to house property (Section 24) is capped at INR 2,00,000." sqref="B37" xr:uid="{ED588459-E29D-4E5A-8541-A348723FCF4B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Deductions under Section 10" prompt="Deductions under Section 10 include the available benefits in the Old Tax Regime, excluding the Section 10(14) benefits - which can be claimed in the next input." sqref="B38" xr:uid="{05F09584-2384-42B3-A1B7-51A33ED58A78}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Deductions under Section 10(14)" prompt="Deductions under Section 10(14) are the permissible subset of Section 10 deductions in both the tax regimes." sqref="B39 C39" xr:uid="{401BE2A2-98C2-4B8A-935A-C4867BB410B2}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculating tax for income from dividends and capital gains
</commit_message>
<xml_diff>
--- a/src/Tax Simulator.xlsx
+++ b/src/Tax Simulator.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrajvir\Documents\Tax Simulator\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C3B60-FF3A-4021-B85D-5E08877CCDF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F11F0E-2F85-4773-84BE-4BB8CCAA57C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{3843DC55-979D-4730-884A-784DB37EFD9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulator" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
   <si>
     <t>Old Regime</t>
   </si>
@@ -65,9 +68,6 @@
   </si>
   <si>
     <t>Annual Salary</t>
-  </si>
-  <si>
-    <t>PF Contribution (%)</t>
   </si>
   <si>
     <t>Joining Bonus (if applicable)</t>
@@ -191,9 +191,6 @@
     <t>Gross Taxable Income</t>
   </si>
   <si>
-    <t>Gross Taxable income after deductions</t>
-  </si>
-  <si>
     <t>Applicable Income Tax</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>Basic Component + DA (per month)</t>
   </si>
   <si>
-    <t>Employer's PF contirbution is within Annual Salary</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -246,6 +240,53 @@
   </si>
   <si>
     <t>Section 10 deductions</t>
+  </si>
+  <si>
+    <t>Income from Dividends - Foreign Companies (without TDS in foreign country)</t>
+  </si>
+  <si>
+    <t>Section 90 - Tax deducted in foreign countries (with bilateral treaty with India) for dividends</t>
+  </si>
+  <si>
+    <t>Section 91 - Tax deducted in foreign countries (without bilateral treaty with India) for dividends</t>
+  </si>
+  <si>
+    <t>Deductions for interest paid to earn dividends</t>
+  </si>
+  <si>
+    <t>Income from Dividends - Domestic Companies (without TDS)</t>
+  </si>
+  <si>
+    <t>Income from Short Term Capital Gains (applicable under Section 111A)</t>
+  </si>
+  <si>
+    <t>Income from Short Term Capital Gains (NA under Section 111A)</t>
+  </si>
+  <si>
+    <t>Income from Long Term Capital Gains (applicable under Section 112A)</t>
+  </si>
+  <si>
+    <t>Income from Long Term Capital Gains (NA under Section 112A)</t>
+  </si>
+  <si>
+    <t>Income from Long Term Capital Gains (NA under Section 112A, specified assets)
+Select if availing indexation benefit or not</t>
+  </si>
+  <si>
+    <t>PF Contribution (%)
+Select if Employer's PF Contribution is within Annual Salary</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Applicable Income Tax on Capital Gains</t>
+  </si>
+  <si>
+    <t>Total Income Tax after Rebate under Section 87(a)</t>
+  </si>
+  <si>
+    <t>Gross Taxable income after deductions (excluding income under Capital Gains)</t>
   </si>
 </sst>
 </file>
@@ -299,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +360,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -369,7 +416,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -425,11 +472,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFill="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent3" xfId="5" builtinId="37"/>
@@ -450,6 +512,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="IT_CAPITAL_GAINS"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -750,15 +828,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA4E777-56A7-4B35-9A19-002DF34E045D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="62.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.19921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.3984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.1328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.06640625" style="1"/>
@@ -795,20 +873,20 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -822,7 +900,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3">
         <v>43922</v>
@@ -843,7 +921,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -869,12 +947,15 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
-        <v>3</v>
+    <row r="5" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B5" s="1">
         <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="14">
@@ -898,10 +979,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="14">
@@ -925,7 +1006,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -950,7 +1031,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -971,7 +1052,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -993,22 +1074,21 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="13">
-        <f>MIN(B11,MAX(1/4/2020,B3))</f>
-        <v>43922</v>
+      <c r="A10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="G10" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1021,11 +1101,11 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="13">
-        <v>44286</v>
+      <c r="A11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="14"/>
@@ -1042,8 +1122,12 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="14">
         <v>0</v>
@@ -1065,12 +1149,11 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>1</v>
+      <c r="A13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="14">
@@ -1092,15 +1175,15 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="7" t="s">
-        <v>16</v>
+    <row r="14" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>5</v>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="14">
@@ -1124,13 +1207,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>5</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="14">
@@ -1143,9 +1223,6 @@
         <v>0.15</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1153,14 +1230,12 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>5</v>
+      <c r="A16" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="13">
+        <f>MIN(B17,MAX(1/4/2020,B3))</f>
+        <v>43922</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="14">
@@ -1173,9 +1248,6 @@
         <v>0.2</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1183,14 +1255,11 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>5</v>
+      <c r="A17" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="13">
+        <v>44286</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="14">
@@ -1203,9 +1272,6 @@
         <v>0.25</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1213,15 +1279,8 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="14">
         <v>1500000</v>
@@ -1231,9 +1290,6 @@
         <v>0.3</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1241,49 +1297,41 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>5</v>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="8" t="s">
-        <v>9</v>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A20" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1292,24 +1340,21 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1318,17 +1363,17 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -1344,17 +1389,17 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -1370,17 +1415,17 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -1396,18 +1441,15 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1418,20 +1460,17 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="7" t="s">
-        <v>34</v>
+    <row r="26" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1444,18 +1483,15 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1468,18 +1504,15 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1492,18 +1525,15 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="6"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1516,18 +1546,15 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1540,13 +1567,13 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1564,13 +1591,13 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1588,13 +1615,13 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1612,13 +1639,13 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1636,18 +1663,18 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" s="7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -1658,290 +1685,538 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="37" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A38" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A39" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A40" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A41" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+    </row>
+    <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="20">
+        <v>0</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="20">
+        <v>0</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="20">
-        <v>0</v>
-      </c>
-      <c r="C37" s="12" t="s">
+      <c r="B45" s="21">
+        <v>0</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="21"/>
+      <c r="C46" s="9"/>
+    </row>
+    <row r="47" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" s="2" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+      <c r="C49" s="23"/>
+    </row>
+    <row r="50" spans="1:8" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
+      <c r="C50" s="23"/>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="22">
+        <v>0</v>
+      </c>
+      <c r="C51" s="23"/>
+    </row>
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A52"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="23"/>
+    </row>
+    <row r="53" spans="1:8" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="11"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="12"/>
+    </row>
+    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="11"/>
+      <c r="B55" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="10">
+        <f>ROUND((B5/100*B2)*((DATEDIF(B16,EOMONTH(B16,0),"d")+1)/DAY(EOMONTH(B16,0))),0)+ROUND((B5/100*B2)*DATEDIF(B16,B17,"m"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="10">
+        <f>ROUND((B5/100*B2)*((DATEDIF(B16,EOMONTH(B16,0),"d")+1)/DAY(EOMONTH(B16,0))),0)+ROUND((B5/100*B2)*DATEDIF(B16,B17,"m"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="10">
+        <f>IF(B6&gt;B5,ROUND(((B6-B5)/100*B2)*((DATEDIF(B16,EOMONTH(B16,0),"d")+1)/DAY(EOMONTH(B16,0))),0)+ROUND(((B6-B5)/100*B2)*DATEDIF(B16,B17,"m"),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C57" s="10">
+        <f>IF(B6&gt;B5,ROUND(((B6-B5)/100*B2)*((DATEDIF(B16,EOMONTH(B16,0),"d")+1)/DAY(EOMONTH(B16,0))),0)+ROUND(((B6-B5)/100*B2)*DATEDIF(B16,B17,"m"),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="10">
+        <f>ROUND((ROUND((((DATEDIF(B16,EOMONTH(B16,0),"d")+1)/DAY(EOMONTH(B16,0)))*B1/12),0)+ROUND(DATEDIF(B16,B17,"m")*B1/12,0)+B4+B7+IF(B8&gt;5000,0.925*B8,B8)+B9+B11+B15)+IF(C5="Yes",-1*B56,0)-B51,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C58" s="10">
+        <f>ROUND((ROUND((((DATEDIF(B16,EOMONTH(B16,0),"d")+1)/DAY(EOMONTH(B16,0)))*B1/12),0)+ROUND(DATEDIF(B16,B17,"m")*B1/12,0)+B4+B7+IF(B8&gt;5000,0.925*B8,B8)+B9+B11+B15)+IF(C5="Yes",-1*C56,0)-B51,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+    </row>
+    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="20">
-        <v>0</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="22">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="10">
-        <f>ROUND((B5/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND((B5/100*B2)*DATEDIF(B10,B11,"m"),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="10">
-        <f>ROUND((B5/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND((B5/100*B2)*DATEDIF(B10,B11,"m"),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="10">
-        <f>IF(B7&gt;B5,ROUND(((B7-B5)/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND(((B7-B5)/100*B2)*DATEDIF(B10,B11,"m"),0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C42" s="10">
-        <f>IF(B7&gt;B5,ROUND(((B7-B5)/100*B2)*((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0))),0)+ROUND(((B7-B5)/100*B2)*DATEDIF(B10,B11,"m"),0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="18" t="s">
+      <c r="B60" s="11">
+        <v>50000</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="11">
+        <f>MIN(150000,B24+B56+B57)</f>
+        <v>0</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="5"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="11">
+        <f>MIN(50000,B25)+MIN(25000,B26)+MIN(25000,B27)+MIN(50000,B28)+MIN(75000,B29)+MIN(125000,B30)+MIN(40000,B31)+MIN(100000,B32)+B33+MIN(50000,B34)+MIN(150000,B35)+MIN(150000,B36)+B37+MIN(10000,B38)+MIN(50000,B39)+MIN(75000,B40)+MIN(125000,B41)</f>
+        <v>0</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B63" s="11">
+        <f>MIN(200000,B43)</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" s="11">
+        <f>SUM(B44:B45)</f>
+        <v>0</v>
+      </c>
+      <c r="C64" s="12">
+        <f>C45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="10">
+        <f>MAX(0,B58-SUM(B60:B64)-SUM(B20:B23))</f>
+        <v>0</v>
+      </c>
+      <c r="C66" s="10">
+        <f>MAX(0,C58-C64)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="10">
-        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*B41,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C43" s="10">
-        <f>ROUND((ROUND((((DATEDIF(B10,EOMONTH(B10,0),"d")+1)/DAY(EOMONTH(B10,0)))*B1/12),0)+ROUND(DATEDIF(B10,B11,"m")*B1/12,0)+B4+B8+B9)+IF(B6="Yes",-1*C41,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="11">
-        <v>50000</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="11">
-        <f>MIN(150000,B18+B41+B42)</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="11">
-        <f>MIN(50000,B19)+MIN(25000,B20)+MIN(25000,B21)+MIN(50000,B22)+MIN(75000,B23)+MIN(125000,B24)+MIN(40000,B25)+MIN(100000,B26)+B27+MIN(50000,B28)+MIN(150000,B29)+MIN(150000,B30)+B31+MIN(10000,B32)+MIN(50000,B33)+MIN(75000,B34)+MIN(125000,B35)</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="11">
-        <f>MIN(200000,B37)</f>
-        <v>0</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="11">
-        <f>SUM(B38:B39)</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="12">
-        <f>C39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="18" t="s">
+      <c r="B67" s="11" cm="1">
+        <f t="array" ref="B67">ROUND(SUMPRODUCT(G4:G7-G3:G6,B66-E4:E7,N(B66&gt;E4:E7)),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C67" s="11" cm="1">
+        <f t="array" ref="C67">ROUND(SUMPRODUCT(G12:G18-G11:G17,C66-E12:E18,N(C66&gt;E12:E18)),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="11" cm="1">
+        <f t="array" ref="B68">[1]!IT_CAPITAL_GAINS(F4,B66,B10,B12,B13,B14,C14)</f>
+        <v>0</v>
+      </c>
+      <c r="C68" s="11" cm="1">
+        <f t="array" ref="C68">[1]!IT_CAPITAL_GAINS(F12,C66,B10,B12,B13,B14,C14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="11">
+        <f>IF(B66+B10+B12+B13+B14&lt;=F5,MAX(0,B67+B68-((F5-E5)*G5)),B67+B68)</f>
+        <v>0</v>
+      </c>
+      <c r="C69" s="11">
+        <f>IF(C66+B10+B12+B13+B14&lt;=F13,MAX(0,C67+C68-((F13-E13)*G13)),C67+C68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" s="11">
+        <f>IF(B66+B10+B12+B13+B14&lt;5000000,0,IF(B66+B10+B12+B13+B14&lt;=10000000,0.1*B69,IF(B66+B10+B12+B13+B14&lt;=20000000,0.15*B69,IF(B66+B10+B12+B13+B14&lt;=50000000,0.25*B69,0.37*B69))))</f>
+        <v>0</v>
+      </c>
+      <c r="C70" s="11">
+        <f>IF(C66+B10+B12+B13+B14&lt;5000000,0,IF(C66+B10+B12+B13+B14&lt;=10000000,0.1*C69,IF(C66+B10+B12+B13+B14&lt;=20000000,0.15*C69,IF(C66+B10+B12+B13+B14&lt;=50000000,0.25*C69,0.37*C69))))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="10">
-        <f>MAX(0,B43-SUM(B44:B48)-SUM(B14:B17))</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="10">
-        <f>MAX(0,C43-C48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="11" cm="1">
-        <f t="array" ref="B51">ROUND(IF(B50&gt;500000,SUMPRODUCT(G4:G7-G3:G6,B50-E4:E7,N(B50&gt;E4:E7)),0),2)</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="11" cm="1">
-        <f t="array" ref="C51">ROUND(IF(C50&gt;500000,SUMPRODUCT(G12:G18-G11:G17,C50-E12:E18,N(C50&gt;E12:E18)),0),2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B52" s="11">
-        <f>IF(B50&lt;5000000,0,IF(B50&lt;=10000000,0.1*B51,IF(B50&lt;=20000000,0.15*B51,IF(B50&lt;=50000000,0.25*B51,0.37*B51))))</f>
-        <v>0</v>
-      </c>
-      <c r="C52" s="11">
-        <f>IF(C50&lt;5000000,0,IF(C50&lt;=10000000,0.1*C51,IF(C50&lt;=20000000,0.15*C51,IF(C50&lt;=50000000,0.25*C51,0.37*C51))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="18" t="s">
+      <c r="B71" s="11">
+        <f>0.04*(B69+B70)</f>
+        <v>0</v>
+      </c>
+      <c r="C71" s="11">
+        <f>0.04*(C69+C70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="11">
-        <f>0.04*(B51+B52)</f>
-        <v>0</v>
-      </c>
-      <c r="C53" s="11">
-        <f>0.04*(C51+C52)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="11">
-        <f>ROUND(SUM(B51:B53),2)</f>
-        <v>0</v>
-      </c>
-      <c r="C54" s="11">
-        <f>ROUND(SUM(C51:C53),2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A56" s="19" t="s">
+      <c r="B72" s="11">
+        <f>ROUND(MAX(0,SUM(B69:B71)-SUM(B49:B50)),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C72" s="11">
+        <f>ROUND(MAX(0,SUM(C69:C71)-SUM(C49:C50)),2)</f>
+        <v>0</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+    </row>
+    <row r="74" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="75" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="26"/>
+      <c r="B75" s="27"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A76" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76" s="11">
+        <f>ROUND(ABS(B72-C72),2)</f>
+        <v>0</v>
+      </c>
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A77" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B56" s="11">
-        <f>ROUND(ABS(B54-C54),2)</f>
-        <v>0</v>
-      </c>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A57" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="12" t="str">
-        <f>IF(B54&gt;C54,"New Regime", "Old Regime")</f>
+      <c r="B77" s="12" t="str">
+        <f>IF(B72&gt;C72,"New Regime", "Old Regime")</f>
         <v>Old Regime</v>
       </c>
-      <c r="C57" s="2"/>
+      <c r="C77" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rwmyt6hHFpYmvFLcvmcX67p6pfpbl+rOXDJj/5Rs0Rz96jO2/hYXq6KmCdxUW8xLjBKV6kIhqWWw+5ZMJQpJIQ==" saltValue="iq/Ekhjv1Lh2pW3nyEiDOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="1">
-    <mergeCell ref="A55:XFD55"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="EXCeWn4Cil7RREEeIpKDNJgPaGea+omeSbNKmigVHK2NVBz1Xht3EuqN03k6SxdnIy3ltd/i9jiku63m/6qvsg==" saltValue="HOSUJDSVXV0KgVX/tLtUdA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A74:XFD74"/>
+    <mergeCell ref="A47:XFD47"/>
+    <mergeCell ref="A53:XFD53"/>
   </mergeCells>
-  <dataValidations xWindow="794" yWindow="922" count="17">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Housing Loan Benefit" error="Section 80EEA benefit is applicable only when benefit is not claimed under Section 80EE._x000a_" sqref="B29" xr:uid="{9996CA8A-1186-40D8-8322-5EEC3D7CD6F5}">
+  <dataValidations xWindow="794" yWindow="922" count="22">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Housing Loan Benefit" error="Section 80EEA benefit is applicable only when benefit is not claimed under Section 80EE._x000a_" sqref="B35" xr:uid="{9996CA8A-1186-40D8-8322-5EEC3D7CD6F5}">
+      <formula1>$B$34=0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="80D Parents (Sr. Citizens)" error="Claims under Section 80D Parents (Sr. Citizens) is mutually exclusive to claims under Section 80D Parents." sqref="B28" xr:uid="{172527D4-8EC9-4EB1-9456-81AF2B9B8E4D}">
+      <formula1>$B$27=0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80D Parents" error="Claims under Section 80D Parents (Sr. Citizens) is mutually exclusive to claims under Section 80D Parents." sqref="B27" xr:uid="{D19E5B0F-4CA7-4186-8345-EE1C810E8352}">
       <formula1>$B$28=0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="80D Parents (Sr. Citizens)" error="Claims under Section 80D Parents (Sr. Citizens) is mutually exclusive to claims under Section 80D Parents." sqref="B22" xr:uid="{172527D4-8EC9-4EB1-9456-81AF2B9B8E4D}">
-      <formula1>$B$21=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80D Parents" error="Claims under Section 80D Parents (Sr. Citizens) is mutually exclusive to claims under Section 80D Parents." sqref="B21" xr:uid="{D19E5B0F-4CA7-4186-8345-EE1C810E8352}">
-      <formula1>$B$22=0</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPF Contribution" error="VPF Contribution is the additional % of (Basic + DA income), over EPF rate, allocated to be contibuted to the PF account." sqref="B7" xr:uid="{B99E13DA-B108-4CD9-BDE5-42885B96B457}">
-      <formula1>IF($B$7&gt;0,$B$5,0)</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPF Contribution" error="VPF Contribution is the additional % of (Basic + DA income), over EPF rate, allocated to be contibuted to the PF account." sqref="B6" xr:uid="{B99E13DA-B108-4CD9-BDE5-42885B96B457}">
+      <formula1>IF($B$6&gt;0,$B$5,0)</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80U - Self disability" error="Deductions under Section 80U and Section 80DD are mutually exclusive." sqref="B34" xr:uid="{2E7F7CD0-CE0B-4653-A4BE-060C657EBBC0}">
-      <formula1>AND($B$23=0,$B$24=0)</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80U - Self disability" error="Deductions under Section 80U and Section 80DD are mutually exclusive." sqref="B40" xr:uid="{2E7F7CD0-CE0B-4653-A4BE-060C657EBBC0}">
+      <formula1>AND($B$29=0,$B$30=0)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80U" error="Deductions under Section 80U and Section 80DD are mutually exclusive." sqref="B35" xr:uid="{562C85F8-6F64-4522-94E9-686B33A3AE20}">
-      <formula1>AND($B$23=0,$B$24=0)</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80U" error="Deductions under Section 80U and Section 80DD are mutually exclusive." sqref="B41" xr:uid="{562C85F8-6F64-4522-94E9-686B33A3AE20}">
+      <formula1>AND($B$29=0,$B$30=0)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80DD " error="Claims under Section 80DD and Section 80U are mutually exclusive for deductions." sqref="B23" xr:uid="{67A206C9-61DF-4D7B-BBE8-19A0286871A9}">
-      <formula1>AND($B$34=0,$B$35=0)</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80DD " error="Claims under Section 80DD and Section 80U are mutually exclusive for deductions." sqref="B29" xr:uid="{67A206C9-61DF-4D7B-BBE8-19A0286871A9}">
+      <formula1>AND($B$40=0,$B$41=0)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80DD" error="Claims under Section 80DD and Section 80U are mutually exclusive for deductions." sqref="B24" xr:uid="{B9F57AA7-51BA-4BEA-B5C3-EE9C9138BD62}">
-      <formula1>AND($B$34=0,$B$35=0)</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Section 80DD" error="Claims under Section 80DD and Section 80U are mutually exclusive for deductions." sqref="B30" xr:uid="{B9F57AA7-51BA-4BEA-B5C3-EE9C9138BD62}">
+      <formula1>AND($B$40=0,$B$41=0)</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Children's Edu.+Hostel Allowance" error="Children's education allowance is capped at INR 100 per month per child for upto 2 children AND hostel allowance is capped at INR 300 per month per child for upto 2 children." promptTitle="Children's Edu.+Hostel Allowance" prompt="Children's Education Allowance can be availed at INR 100 per month and Children's Hostel Allowance can be availed at INR 300 per month, each upto maximum of 2 children." sqref="B17" xr:uid="{7E32C0C2-BDF6-4A15-B0C9-BC5BC182BAED}">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Children's Edu.+Hostel Allowance" error="Children's education allowance is capped at INR 100 per month per child for upto 2 children AND hostel allowance is capped at INR 300 per month per child for upto 2 children." promptTitle="Children's Edu.+Hostel Allowance" prompt="Children's Education Allowance can be availed at INR 100 per month and Children's Hostel Allowance can be availed at INR 300 per month, each upto maximum of 2 children." sqref="B23" xr:uid="{7E32C0C2-BDF6-4A15-B0C9-BC5BC182BAED}">
       <formula1>9600</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Basic Component" error="Basic Component per month can be set maximum to salary per month (i.e. annual salary / 12)." sqref="B2" xr:uid="{C850F721-3530-449B-BDFF-676D1C665B56}">
       <formula1>($B$1/12)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{8E20BC2B-EF98-449D-A2E2-E47FFC415F51}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Section 80C deductions" prompt="The benefits under Section 80C will be capped at INR 1,50,000 in the tax calculations for old regime." sqref="B18" xr:uid="{143DAB20-1D1B-4AD9-AF0B-8274C33D7380}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Section 80C deductions" prompt="The benefits under Section 80C will be capped at INR 1,50,000 in the tax calculations for old regime." sqref="B24" xr:uid="{143DAB20-1D1B-4AD9-AF0B-8274C33D7380}"/>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PF Contribution Rate" error="The rate of contribution to PF account must be greater than or equal to 0." sqref="B5" xr:uid="{7C1574A4-DCA6-4257-B236-8AE4BA85C4E1}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Housing loan benefit" error="Section 80EEA benefit is applicable only when benefit is not claimed under Section 80EE._x000a_" sqref="B28" xr:uid="{F90C388A-3E0D-4710-A78E-B724F22E5850}">
-      <formula1>$B$29=0</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Housing loan benefit" error="Section 80EEA benefit is applicable only when benefit is not claimed under Section 80EE._x000a_" sqref="B34" xr:uid="{F90C388A-3E0D-4710-A78E-B724F22E5850}">
+      <formula1>$B$35=0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Loss from House Property" prompt="Deductions under loss of income due to house property (Section 24) is capped at INR 2,00,000." sqref="B37" xr:uid="{ED588459-E29D-4E5A-8541-A348723FCF4B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Deductions under Section 10" prompt="Deductions under Section 10 include the available benefits in the Old Tax Regime, excluding the Section 10(14) benefits - which can be claimed in the next input." sqref="B38" xr:uid="{05F09584-2384-42B3-A1B7-51A33ED58A78}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Deductions under Section 10(14)" prompt="Deductions under Section 10(14) are the permissible subset of Section 10 deductions in both the tax regimes." sqref="B39 C39" xr:uid="{401BE2A2-98C2-4B8A-935A-C4867BB410B2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Loss from House Property" prompt="Deductions under loss of income due to house property (Section 24) is capped at INR 2,00,000." sqref="B43" xr:uid="{ED588459-E29D-4E5A-8541-A348723FCF4B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Deductions under Section 10" prompt="Deductions under Section 10 include the available benefits in the Old Tax Regime, excluding the Section 10(14) benefits - which can be claimed in the next input." sqref="B44" xr:uid="{05F09584-2384-42B3-A1B7-51A33ED58A78}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Deductions under Section 10(14)" prompt="Deductions under Section 10(14) are the permissible subset of Section 10 deductions in both the tax regimes." sqref="B45:C46" xr:uid="{401BE2A2-98C2-4B8A-935A-C4867BB410B2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Section 90 deductions" prompt="Section 90 deductions are useful in saving Double Tax payment for the dividends earned from foreign with whom India has signed the DTAA treaty. Tax deducted in foreign country can be completely exempted from tax in India. " sqref="B49" xr:uid="{DC79ED96-E6EA-4DA8-919E-191790780135}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Section 91 deductions" prompt="Section 91 deductions are useful in saving Double Tax payment for the dividends earned from foreign with whom India does not have the DTAA signed. Although, tax deducted in foreign country can be exempted from tax in India, based on specific IT rules." sqref="B50" xr:uid="{116FE396-B12D-4759-B6F2-EC2C5A70AB9C}"/>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Deductions for earning dividends" error="Deductions for interest paid in earning dividends is capped at 20% of Gross Dividend Income, i.e. Domestic + Foreign." promptTitle="Deductions for earning dividends" prompt="Deductions can claimed for any interest paid on the amount borrowed for earning divideds. It is capped at 20% of Gross Dividend Income, i.e. Domestic + Foreign." sqref="B54 B51" xr:uid="{6208C941-2510-44C5-88CD-7735E0024810}">
+      <formula1>0.2*($B$8+$B$9)</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Income from Dividends" prompt="Income from Dividends - Domestic Companies is taxed at normal slab rates in the hands of individual taxpayers starting FY 2020-2021 and the TDS deducted (by the domestic company) for AY 2020-2021 will be 7.5%." sqref="B8" xr:uid="{0D2D4AF3-89C9-43D3-89F3-00E0D0290349}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Income from Dividends" prompt="Income from Dividends - Foreign Companies is taxed as per normal slab rates. Deductions for tax paid to foreign company can be claimed under Section 90 and 91 to save double taxation." sqref="B9" xr:uid="{2D2232F0-0A1C-4FBE-99ED-B5144499B427}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 C5" xr:uid="{674BABF6-E2D6-4CAE-A14B-2B20B0423838}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>